<commit_message>
fixed the annual income column
</commit_message>
<xml_diff>
--- a/data/sample.xlsx
+++ b/data/sample.xlsx
@@ -1,26 +1,42 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\data\a11\sessions\day_2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\data\a11\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9499C7B9-B78A-4B37-A5FE-CECE892DF964}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B772158B-FD84-49EE-8277-49FB80DA0853}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1116" yWindow="1116" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1464" yWindow="1464" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <externalReferences>
+    <externalReference r:id="rId2"/>
+  </externalReferences>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="500" uniqueCount="159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="499" uniqueCount="158">
   <si>
     <t>name</t>
   </si>
@@ -494,9 +510,6 @@
   </si>
   <si>
     <t>Charles Johnson</t>
-  </si>
-  <si>
-    <t>yearly_income</t>
   </si>
 </sst>
 </file>
@@ -572,6 +585,523 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <xxl21:alternateUrls>
+      <xxl21:absoluteUrl r:id="rId2"/>
+    </xxl21:alternateUrls>
+    <sheetNames>
+      <sheetName val="Sheet1"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0">
+        <row r="1">
+          <cell r="B1" t="str">
+            <v>annual_income</v>
+          </cell>
+        </row>
+        <row r="2">
+          <cell r="B2">
+            <v>35417</v>
+          </cell>
+        </row>
+        <row r="3">
+          <cell r="B3">
+            <v>21758</v>
+          </cell>
+        </row>
+        <row r="4">
+          <cell r="B4">
+            <v>14792</v>
+          </cell>
+        </row>
+        <row r="5">
+          <cell r="B5">
+            <v>49696</v>
+          </cell>
+        </row>
+        <row r="6">
+          <cell r="B6">
+            <v>42602</v>
+          </cell>
+        </row>
+        <row r="7">
+          <cell r="B7">
+            <v>38600</v>
+          </cell>
+        </row>
+        <row r="8">
+          <cell r="B8">
+            <v>18330</v>
+          </cell>
+        </row>
+        <row r="9">
+          <cell r="B9">
+            <v>35676</v>
+          </cell>
+        </row>
+        <row r="10">
+          <cell r="B10">
+            <v>20515</v>
+          </cell>
+        </row>
+        <row r="11">
+          <cell r="B11">
+            <v>20128</v>
+          </cell>
+        </row>
+        <row r="12">
+          <cell r="B12">
+            <v>34781</v>
+          </cell>
+        </row>
+        <row r="13">
+          <cell r="B13">
+            <v>26728</v>
+          </cell>
+        </row>
+        <row r="14">
+          <cell r="B14">
+            <v>50958</v>
+          </cell>
+        </row>
+        <row r="15">
+          <cell r="B15">
+            <v>35147</v>
+          </cell>
+        </row>
+        <row r="16">
+          <cell r="B16">
+            <v>31153</v>
+          </cell>
+        </row>
+        <row r="17">
+          <cell r="B17">
+            <v>48302</v>
+          </cell>
+        </row>
+        <row r="18">
+          <cell r="B18">
+            <v>42824</v>
+          </cell>
+        </row>
+        <row r="19">
+          <cell r="B19">
+            <v>49399</v>
+          </cell>
+        </row>
+        <row r="20">
+          <cell r="B20">
+            <v>51077</v>
+          </cell>
+        </row>
+        <row r="21">
+          <cell r="B21">
+            <v>48378</v>
+          </cell>
+        </row>
+        <row r="22">
+          <cell r="B22">
+            <v>28728</v>
+          </cell>
+        </row>
+        <row r="23">
+          <cell r="B23">
+            <v>46284</v>
+          </cell>
+        </row>
+        <row r="24">
+          <cell r="B24">
+            <v>50178</v>
+          </cell>
+        </row>
+        <row r="25">
+          <cell r="B25">
+            <v>23834</v>
+          </cell>
+        </row>
+        <row r="26">
+          <cell r="B26">
+            <v>43930</v>
+          </cell>
+        </row>
+        <row r="27">
+          <cell r="B27">
+            <v>52868</v>
+          </cell>
+        </row>
+        <row r="28">
+          <cell r="B28">
+            <v>13797</v>
+          </cell>
+        </row>
+        <row r="29">
+          <cell r="B29">
+            <v>56362</v>
+          </cell>
+        </row>
+        <row r="30">
+          <cell r="B30">
+            <v>64065</v>
+          </cell>
+        </row>
+        <row r="31">
+          <cell r="B31">
+            <v>44015</v>
+          </cell>
+        </row>
+        <row r="32">
+          <cell r="B32">
+            <v>60608</v>
+          </cell>
+        </row>
+        <row r="33">
+          <cell r="B33">
+            <v>15406</v>
+          </cell>
+        </row>
+        <row r="34">
+          <cell r="B34">
+            <v>56529</v>
+          </cell>
+        </row>
+        <row r="35">
+          <cell r="B35">
+            <v>16435</v>
+          </cell>
+        </row>
+        <row r="36">
+          <cell r="B36">
+            <v>27204</v>
+          </cell>
+        </row>
+        <row r="37">
+          <cell r="B37">
+            <v>39856</v>
+          </cell>
+        </row>
+        <row r="38">
+          <cell r="B38">
+            <v>51414</v>
+          </cell>
+        </row>
+        <row r="39">
+          <cell r="B39">
+            <v>40329</v>
+          </cell>
+        </row>
+        <row r="40">
+          <cell r="B40">
+            <v>50694</v>
+          </cell>
+        </row>
+        <row r="41">
+          <cell r="B41">
+            <v>45931</v>
+          </cell>
+        </row>
+        <row r="42">
+          <cell r="B42">
+            <v>19405</v>
+          </cell>
+        </row>
+        <row r="43">
+          <cell r="B43">
+            <v>19387</v>
+          </cell>
+        </row>
+        <row r="44">
+          <cell r="B44">
+            <v>20823</v>
+          </cell>
+        </row>
+        <row r="45">
+          <cell r="B45">
+            <v>33529</v>
+          </cell>
+        </row>
+        <row r="46">
+          <cell r="B46">
+            <v>53766</v>
+          </cell>
+        </row>
+        <row r="47">
+          <cell r="B47">
+            <v>31129</v>
+          </cell>
+        </row>
+        <row r="48">
+          <cell r="B48">
+            <v>27650</v>
+          </cell>
+        </row>
+        <row r="49">
+          <cell r="B49">
+            <v>29589</v>
+          </cell>
+        </row>
+        <row r="50">
+          <cell r="B50">
+            <v>51031</v>
+          </cell>
+        </row>
+        <row r="51">
+          <cell r="B51">
+            <v>47613</v>
+          </cell>
+        </row>
+        <row r="52">
+          <cell r="B52">
+            <v>50238</v>
+          </cell>
+        </row>
+        <row r="53">
+          <cell r="B53">
+            <v>28008</v>
+          </cell>
+        </row>
+        <row r="54">
+          <cell r="B54">
+            <v>53556</v>
+          </cell>
+        </row>
+        <row r="55">
+          <cell r="B55">
+            <v>41606</v>
+          </cell>
+        </row>
+        <row r="56">
+          <cell r="B56">
+            <v>22606</v>
+          </cell>
+        </row>
+        <row r="57">
+          <cell r="B57">
+            <v>48153</v>
+          </cell>
+        </row>
+        <row r="58">
+          <cell r="B58">
+            <v>38608</v>
+          </cell>
+        </row>
+        <row r="59">
+          <cell r="B59">
+            <v>45881</v>
+          </cell>
+        </row>
+        <row r="60">
+          <cell r="B60">
+            <v>27368</v>
+          </cell>
+        </row>
+        <row r="61">
+          <cell r="B61">
+            <v>46232</v>
+          </cell>
+        </row>
+        <row r="62">
+          <cell r="B62">
+            <v>41239</v>
+          </cell>
+        </row>
+        <row r="63">
+          <cell r="B63">
+            <v>23632</v>
+          </cell>
+        </row>
+        <row r="64">
+          <cell r="B64">
+            <v>31265</v>
+          </cell>
+        </row>
+        <row r="65">
+          <cell r="B65">
+            <v>16891</v>
+          </cell>
+        </row>
+        <row r="66">
+          <cell r="B66">
+            <v>51143</v>
+          </cell>
+        </row>
+        <row r="67">
+          <cell r="B67">
+            <v>48705</v>
+          </cell>
+        </row>
+        <row r="68">
+          <cell r="B68">
+            <v>58720</v>
+          </cell>
+        </row>
+        <row r="69">
+          <cell r="B69">
+            <v>12229</v>
+          </cell>
+        </row>
+        <row r="70">
+          <cell r="B70">
+            <v>25924</v>
+          </cell>
+        </row>
+        <row r="71">
+          <cell r="B71">
+            <v>52449</v>
+          </cell>
+        </row>
+        <row r="72">
+          <cell r="B72">
+            <v>17815</v>
+          </cell>
+        </row>
+        <row r="73">
+          <cell r="B73">
+            <v>54547</v>
+          </cell>
+        </row>
+        <row r="74">
+          <cell r="B74">
+            <v>57726</v>
+          </cell>
+        </row>
+        <row r="75">
+          <cell r="B75">
+            <v>38422</v>
+          </cell>
+        </row>
+        <row r="76">
+          <cell r="B76">
+            <v>50047</v>
+          </cell>
+        </row>
+        <row r="77">
+          <cell r="B77">
+            <v>15710</v>
+          </cell>
+        </row>
+        <row r="78">
+          <cell r="B78">
+            <v>61943</v>
+          </cell>
+        </row>
+        <row r="79">
+          <cell r="B79">
+            <v>53000</v>
+          </cell>
+        </row>
+        <row r="80">
+          <cell r="B80">
+            <v>23927</v>
+          </cell>
+        </row>
+        <row r="81">
+          <cell r="B81">
+            <v>11130</v>
+          </cell>
+        </row>
+        <row r="82">
+          <cell r="B82">
+            <v>13763</v>
+          </cell>
+        </row>
+        <row r="83">
+          <cell r="B83">
+            <v>30465</v>
+          </cell>
+        </row>
+        <row r="84">
+          <cell r="B84">
+            <v>46710</v>
+          </cell>
+        </row>
+        <row r="85">
+          <cell r="B85">
+            <v>14721</v>
+          </cell>
+        </row>
+        <row r="86">
+          <cell r="B86">
+            <v>63836</v>
+          </cell>
+        </row>
+        <row r="87">
+          <cell r="B87">
+            <v>35245</v>
+          </cell>
+        </row>
+        <row r="88">
+          <cell r="B88">
+            <v>37009</v>
+          </cell>
+        </row>
+        <row r="89">
+          <cell r="B89">
+            <v>47365</v>
+          </cell>
+        </row>
+        <row r="90">
+          <cell r="B90">
+            <v>40802</v>
+          </cell>
+        </row>
+        <row r="91">
+          <cell r="B91">
+            <v>12150</v>
+          </cell>
+        </row>
+        <row r="92">
+          <cell r="B92">
+            <v>31832</v>
+          </cell>
+        </row>
+        <row r="93">
+          <cell r="B93">
+            <v>53719</v>
+          </cell>
+        </row>
+        <row r="94">
+          <cell r="B94">
+            <v>49821</v>
+          </cell>
+        </row>
+        <row r="95">
+          <cell r="B95">
+            <v>10416</v>
+          </cell>
+        </row>
+        <row r="96">
+          <cell r="B96">
+            <v>26356</v>
+          </cell>
+        </row>
+        <row r="97">
+          <cell r="B97">
+            <v>53983</v>
+          </cell>
+        </row>
+        <row r="98">
+          <cell r="B98">
+            <v>43715</v>
+          </cell>
+        </row>
+        <row r="99">
+          <cell r="B99">
+            <v>28048</v>
+          </cell>
+        </row>
+        <row r="100">
+          <cell r="B100">
+            <v>64336</v>
+          </cell>
+        </row>
+      </sheetData>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -861,8 +1391,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G101"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
+      <selection activeCell="G58" sqref="G58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -886,8 +1416,9 @@
       <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>158</v>
+      <c r="G1" s="1" t="str">
+        <f>[1]Sheet1!B1</f>
+        <v>annual_income</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
@@ -909,6 +1440,10 @@
       <c r="F2" t="s">
         <v>10</v>
       </c>
+      <c r="G2">
+        <f>[1]Sheet1!B2</f>
+        <v>35417</v>
+      </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
@@ -929,6 +1464,10 @@
       <c r="F3" t="s">
         <v>10</v>
       </c>
+      <c r="G3">
+        <f>[1]Sheet1!B3</f>
+        <v>21758</v>
+      </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
@@ -949,6 +1488,10 @@
       <c r="F4" t="s">
         <v>15</v>
       </c>
+      <c r="G4">
+        <f>[1]Sheet1!B4</f>
+        <v>14792</v>
+      </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
@@ -969,6 +1512,10 @@
       <c r="F5" t="s">
         <v>10</v>
       </c>
+      <c r="G5">
+        <f>[1]Sheet1!B5</f>
+        <v>49696</v>
+      </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
@@ -989,6 +1536,10 @@
       <c r="F6" t="s">
         <v>10</v>
       </c>
+      <c r="G6">
+        <f>[1]Sheet1!B6</f>
+        <v>42602</v>
+      </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
@@ -1009,6 +1560,10 @@
       <c r="F7" t="s">
         <v>15</v>
       </c>
+      <c r="G7">
+        <f>[1]Sheet1!B7</f>
+        <v>38600</v>
+      </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
@@ -1029,6 +1584,10 @@
       <c r="F8" t="s">
         <v>10</v>
       </c>
+      <c r="G8">
+        <f>[1]Sheet1!B8</f>
+        <v>18330</v>
+      </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
@@ -1049,6 +1608,10 @@
       <c r="F9" t="s">
         <v>10</v>
       </c>
+      <c r="G9">
+        <f>[1]Sheet1!B9</f>
+        <v>35676</v>
+      </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
@@ -1069,6 +1632,10 @@
       <c r="F10" t="s">
         <v>15</v>
       </c>
+      <c r="G10">
+        <f>[1]Sheet1!B10</f>
+        <v>20515</v>
+      </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
@@ -1089,6 +1656,10 @@
       <c r="F11" t="s">
         <v>10</v>
       </c>
+      <c r="G11">
+        <f>[1]Sheet1!B11</f>
+        <v>20128</v>
+      </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
@@ -1109,6 +1680,10 @@
       <c r="F12" t="s">
         <v>15</v>
       </c>
+      <c r="G12">
+        <f>[1]Sheet1!B12</f>
+        <v>34781</v>
+      </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
@@ -1129,6 +1704,10 @@
       <c r="F13" t="s">
         <v>10</v>
       </c>
+      <c r="G13">
+        <f>[1]Sheet1!B13</f>
+        <v>26728</v>
+      </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
@@ -1146,6 +1725,10 @@
       <c r="F14" t="s">
         <v>15</v>
       </c>
+      <c r="G14">
+        <f>[1]Sheet1!B14</f>
+        <v>50958</v>
+      </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
@@ -1166,6 +1749,10 @@
       <c r="F15" t="s">
         <v>10</v>
       </c>
+      <c r="G15">
+        <f>[1]Sheet1!B15</f>
+        <v>35147</v>
+      </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
@@ -1186,8 +1773,12 @@
       <c r="F16" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G16">
+        <f>[1]Sheet1!B16</f>
+        <v>31153</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>42</v>
       </c>
@@ -1206,8 +1797,12 @@
       <c r="F17" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G17">
+        <f>[1]Sheet1!B17</f>
+        <v>48302</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>44</v>
       </c>
@@ -1226,8 +1821,12 @@
       <c r="F18" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G18">
+        <f>[1]Sheet1!B18</f>
+        <v>42824</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>46</v>
       </c>
@@ -1246,8 +1845,12 @@
       <c r="F19" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G19">
+        <f>[1]Sheet1!B19</f>
+        <v>49399</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>48</v>
       </c>
@@ -1266,8 +1869,12 @@
       <c r="F20" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G20">
+        <f>[1]Sheet1!B20</f>
+        <v>51077</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>50</v>
       </c>
@@ -1286,8 +1893,12 @@
       <c r="F21" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G21">
+        <f>[1]Sheet1!B21</f>
+        <v>48378</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>53</v>
       </c>
@@ -1306,8 +1917,12 @@
       <c r="F22" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G22">
+        <f>[1]Sheet1!B22</f>
+        <v>28728</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>55</v>
       </c>
@@ -1326,8 +1941,12 @@
       <c r="F23" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G23">
+        <f>[1]Sheet1!B23</f>
+        <v>46284</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>56</v>
       </c>
@@ -1346,8 +1965,12 @@
       <c r="F24" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G24">
+        <f>[1]Sheet1!B24</f>
+        <v>50178</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>57</v>
       </c>
@@ -1366,8 +1989,12 @@
       <c r="F25" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G25">
+        <f>[1]Sheet1!B25</f>
+        <v>23834</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>58</v>
       </c>
@@ -1386,8 +2013,12 @@
       <c r="F26" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G26">
+        <f>[1]Sheet1!B26</f>
+        <v>43930</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>59</v>
       </c>
@@ -1403,8 +2034,12 @@
       <c r="E27" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G27">
+        <f>[1]Sheet1!B27</f>
+        <v>52868</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>61</v>
       </c>
@@ -1423,8 +2058,12 @@
       <c r="F28" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G28">
+        <f>[1]Sheet1!B28</f>
+        <v>13797</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>62</v>
       </c>
@@ -1443,8 +2082,12 @@
       <c r="F29" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G29">
+        <f>[1]Sheet1!B29</f>
+        <v>56362</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>64</v>
       </c>
@@ -1463,8 +2106,12 @@
       <c r="F30" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G30">
+        <f>[1]Sheet1!B30</f>
+        <v>64065</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>66</v>
       </c>
@@ -1483,8 +2130,12 @@
       <c r="F31" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G31">
+        <f>[1]Sheet1!B31</f>
+        <v>44015</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>67</v>
       </c>
@@ -1503,8 +2154,12 @@
       <c r="F32" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G32">
+        <f>[1]Sheet1!B32</f>
+        <v>60608</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>68</v>
       </c>
@@ -1523,8 +2178,12 @@
       <c r="F33" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G33">
+        <f>[1]Sheet1!B33</f>
+        <v>15406</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>70</v>
       </c>
@@ -1543,8 +2202,12 @@
       <c r="F34" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G34">
+        <f>[1]Sheet1!B34</f>
+        <v>56529</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>71</v>
       </c>
@@ -1563,8 +2226,12 @@
       <c r="F35" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G35">
+        <f>[1]Sheet1!B35</f>
+        <v>16435</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>73</v>
       </c>
@@ -1583,8 +2250,12 @@
       <c r="F36" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G36">
+        <f>[1]Sheet1!B36</f>
+        <v>27204</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>75</v>
       </c>
@@ -1603,8 +2274,12 @@
       <c r="F37" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G37">
+        <f>[1]Sheet1!B37</f>
+        <v>39856</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>77</v>
       </c>
@@ -1623,8 +2298,12 @@
       <c r="F38" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G38">
+        <f>[1]Sheet1!B38</f>
+        <v>51414</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>79</v>
       </c>
@@ -1643,8 +2322,12 @@
       <c r="F39" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G39">
+        <f>[1]Sheet1!B39</f>
+        <v>40329</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>80</v>
       </c>
@@ -1663,8 +2346,12 @@
       <c r="F40" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G40">
+        <f>[1]Sheet1!B40</f>
+        <v>50694</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>81</v>
       </c>
@@ -1683,8 +2370,12 @@
       <c r="F41" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G41">
+        <f>[1]Sheet1!B41</f>
+        <v>45931</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>82</v>
       </c>
@@ -1703,8 +2394,12 @@
       <c r="F42" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G42">
+        <f>[1]Sheet1!B42</f>
+        <v>19405</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>84</v>
       </c>
@@ -1723,8 +2418,12 @@
       <c r="F43" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G43">
+        <f>[1]Sheet1!B43</f>
+        <v>19387</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>85</v>
       </c>
@@ -1743,8 +2442,12 @@
       <c r="F44" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G44">
+        <f>[1]Sheet1!B44</f>
+        <v>20823</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>86</v>
       </c>
@@ -1763,8 +2466,12 @@
       <c r="F45" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G45">
+        <f>[1]Sheet1!B45</f>
+        <v>33529</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>87</v>
       </c>
@@ -1783,8 +2490,12 @@
       <c r="F46" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G46">
+        <f>[1]Sheet1!B46</f>
+        <v>53766</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>88</v>
       </c>
@@ -1803,8 +2514,12 @@
       <c r="F47" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G47">
+        <f>[1]Sheet1!B47</f>
+        <v>31129</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>89</v>
       </c>
@@ -1823,8 +2538,12 @@
       <c r="F48" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G48">
+        <f>[1]Sheet1!B48</f>
+        <v>27650</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>90</v>
       </c>
@@ -1843,8 +2562,12 @@
       <c r="F49" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G49">
+        <f>[1]Sheet1!B49</f>
+        <v>29589</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>91</v>
       </c>
@@ -1863,8 +2586,12 @@
       <c r="F50" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G50">
+        <f>[1]Sheet1!B50</f>
+        <v>51031</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>92</v>
       </c>
@@ -1883,8 +2610,12 @@
       <c r="F51" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G51">
+        <f>[1]Sheet1!B51</f>
+        <v>47613</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>93</v>
       </c>
@@ -1903,8 +2634,12 @@
       <c r="F52" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G52">
+        <f>[1]Sheet1!B52</f>
+        <v>50238</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>95</v>
       </c>
@@ -1923,8 +2658,12 @@
       <c r="F53" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G53">
+        <f>[1]Sheet1!B53</f>
+        <v>28008</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>96</v>
       </c>
@@ -1943,8 +2682,12 @@
       <c r="F54" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G54">
+        <f>[1]Sheet1!B54</f>
+        <v>53556</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>98</v>
       </c>
@@ -1963,8 +2706,12 @@
       <c r="F55" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G55">
+        <f>[1]Sheet1!B55</f>
+        <v>41606</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>99</v>
       </c>
@@ -1983,8 +2730,12 @@
       <c r="F56" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G56">
+        <f>[1]Sheet1!B56</f>
+        <v>22606</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>101</v>
       </c>
@@ -2003,8 +2754,12 @@
       <c r="F57" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G57">
+        <f>[1]Sheet1!B57</f>
+        <v>48153</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>102</v>
       </c>
@@ -2023,8 +2778,12 @@
       <c r="F58" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G58">
+        <f>[1]Sheet1!B58</f>
+        <v>38608</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>103</v>
       </c>
@@ -2043,8 +2802,12 @@
       <c r="F59" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G59">
+        <f>[1]Sheet1!B59</f>
+        <v>45881</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>105</v>
       </c>
@@ -2063,8 +2826,12 @@
       <c r="F60" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G60">
+        <f>[1]Sheet1!B60</f>
+        <v>27368</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>106</v>
       </c>
@@ -2083,8 +2850,12 @@
       <c r="F61" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G61">
+        <f>[1]Sheet1!B61</f>
+        <v>46232</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>108</v>
       </c>
@@ -2103,8 +2874,12 @@
       <c r="F62" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G62">
+        <f>[1]Sheet1!B62</f>
+        <v>41239</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>110</v>
       </c>
@@ -2123,8 +2898,12 @@
       <c r="F63" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G63">
+        <f>[1]Sheet1!B63</f>
+        <v>23632</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>111</v>
       </c>
@@ -2143,8 +2922,12 @@
       <c r="F64" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G64">
+        <f>[1]Sheet1!B64</f>
+        <v>31265</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>112</v>
       </c>
@@ -2160,8 +2943,12 @@
       <c r="E65" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G65">
+        <f>[1]Sheet1!B65</f>
+        <v>16891</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>113</v>
       </c>
@@ -2180,8 +2967,12 @@
       <c r="F66" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G66">
+        <f>[1]Sheet1!B66</f>
+        <v>51143</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>114</v>
       </c>
@@ -2200,8 +2991,12 @@
       <c r="F67" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G67">
+        <f>[1]Sheet1!B67</f>
+        <v>48705</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>115</v>
       </c>
@@ -2220,8 +3015,12 @@
       <c r="F68" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G68">
+        <f>[1]Sheet1!B68</f>
+        <v>58720</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>117</v>
       </c>
@@ -2240,8 +3039,12 @@
       <c r="F69" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G69">
+        <f>[1]Sheet1!B69</f>
+        <v>12229</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>118</v>
       </c>
@@ -2260,8 +3063,12 @@
       <c r="F70" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G70">
+        <f>[1]Sheet1!B70</f>
+        <v>25924</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>119</v>
       </c>
@@ -2280,8 +3087,12 @@
       <c r="F71" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G71">
+        <f>[1]Sheet1!B71</f>
+        <v>52449</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>120</v>
       </c>
@@ -2300,8 +3111,12 @@
       <c r="F72" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G72">
+        <f>[1]Sheet1!B72</f>
+        <v>17815</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>121</v>
       </c>
@@ -2317,8 +3132,12 @@
       <c r="F73" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G73">
+        <f>[1]Sheet1!B73</f>
+        <v>54547</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>122</v>
       </c>
@@ -2337,8 +3156,12 @@
       <c r="F74" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G74">
+        <f>[1]Sheet1!B74</f>
+        <v>57726</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
         <v>124</v>
       </c>
@@ -2357,8 +3180,12 @@
       <c r="F75" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G75">
+        <f>[1]Sheet1!B75</f>
+        <v>38422</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
         <v>125</v>
       </c>
@@ -2377,8 +3204,12 @@
       <c r="F76" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G76">
+        <f>[1]Sheet1!B76</f>
+        <v>50047</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>126</v>
       </c>
@@ -2397,8 +3228,12 @@
       <c r="F77" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G77">
+        <f>[1]Sheet1!B77</f>
+        <v>15710</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
         <v>127</v>
       </c>
@@ -2417,8 +3252,12 @@
       <c r="F78" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G78">
+        <f>[1]Sheet1!B78</f>
+        <v>61943</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>129</v>
       </c>
@@ -2437,8 +3276,12 @@
       <c r="F79" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G79">
+        <f>[1]Sheet1!B79</f>
+        <v>53000</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
         <v>131</v>
       </c>
@@ -2454,8 +3297,12 @@
       <c r="F80" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G80">
+        <f>[1]Sheet1!B80</f>
+        <v>23927</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
         <v>132</v>
       </c>
@@ -2474,8 +3321,12 @@
       <c r="F81" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G81">
+        <f>[1]Sheet1!B81</f>
+        <v>11130</v>
+      </c>
+    </row>
+    <row r="82" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
         <v>133</v>
       </c>
@@ -2491,8 +3342,12 @@
       <c r="E82" t="s">
         <v>134</v>
       </c>
-    </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G82">
+        <f>[1]Sheet1!B82</f>
+        <v>13763</v>
+      </c>
+    </row>
+    <row r="83" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
         <v>135</v>
       </c>
@@ -2511,8 +3366,12 @@
       <c r="F83" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G83">
+        <f>[1]Sheet1!B83</f>
+        <v>30465</v>
+      </c>
+    </row>
+    <row r="84" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
         <v>136</v>
       </c>
@@ -2531,8 +3390,12 @@
       <c r="F84" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G84">
+        <f>[1]Sheet1!B84</f>
+        <v>46710</v>
+      </c>
+    </row>
+    <row r="85" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
         <v>138</v>
       </c>
@@ -2551,8 +3414,12 @@
       <c r="F85" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G85">
+        <f>[1]Sheet1!B85</f>
+        <v>14721</v>
+      </c>
+    </row>
+    <row r="86" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
         <v>139</v>
       </c>
@@ -2571,8 +3438,12 @@
       <c r="F86" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G86">
+        <f>[1]Sheet1!B86</f>
+        <v>63836</v>
+      </c>
+    </row>
+    <row r="87" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
         <v>140</v>
       </c>
@@ -2591,8 +3462,12 @@
       <c r="F87" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G87">
+        <f>[1]Sheet1!B87</f>
+        <v>35245</v>
+      </c>
+    </row>
+    <row r="88" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
         <v>141</v>
       </c>
@@ -2611,8 +3486,12 @@
       <c r="F88" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G88">
+        <f>[1]Sheet1!B88</f>
+        <v>37009</v>
+      </c>
+    </row>
+    <row r="89" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
         <v>142</v>
       </c>
@@ -2631,8 +3510,12 @@
       <c r="F89" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G89">
+        <f>[1]Sheet1!B89</f>
+        <v>47365</v>
+      </c>
+    </row>
+    <row r="90" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
         <v>143</v>
       </c>
@@ -2651,8 +3534,12 @@
       <c r="F90" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G90">
+        <f>[1]Sheet1!B90</f>
+        <v>40802</v>
+      </c>
+    </row>
+    <row r="91" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
         <v>144</v>
       </c>
@@ -2671,8 +3558,12 @@
       <c r="F91" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G91">
+        <f>[1]Sheet1!B91</f>
+        <v>12150</v>
+      </c>
+    </row>
+    <row r="92" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
         <v>145</v>
       </c>
@@ -2691,8 +3582,12 @@
       <c r="F92" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G92">
+        <f>[1]Sheet1!B92</f>
+        <v>31832</v>
+      </c>
+    </row>
+    <row r="93" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
         <v>146</v>
       </c>
@@ -2711,8 +3606,12 @@
       <c r="F93" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G93">
+        <f>[1]Sheet1!B93</f>
+        <v>53719</v>
+      </c>
+    </row>
+    <row r="94" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
         <v>147</v>
       </c>
@@ -2731,8 +3630,12 @@
       <c r="F94" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G94">
+        <f>[1]Sheet1!B94</f>
+        <v>49821</v>
+      </c>
+    </row>
+    <row r="95" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
         <v>149</v>
       </c>
@@ -2751,8 +3654,12 @@
       <c r="F95" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G95">
+        <f>[1]Sheet1!B95</f>
+        <v>10416</v>
+      </c>
+    </row>
+    <row r="96" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
         <v>151</v>
       </c>
@@ -2771,8 +3678,12 @@
       <c r="F96" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="97" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G96">
+        <f>[1]Sheet1!B96</f>
+        <v>26356</v>
+      </c>
+    </row>
+    <row r="97" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
         <v>153</v>
       </c>
@@ -2791,8 +3702,12 @@
       <c r="F97" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="98" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G97">
+        <f>[1]Sheet1!B97</f>
+        <v>53983</v>
+      </c>
+    </row>
+    <row r="98" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
         <v>154</v>
       </c>
@@ -2811,8 +3726,12 @@
       <c r="F98" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="99" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G98">
+        <f>[1]Sheet1!B98</f>
+        <v>43715</v>
+      </c>
+    </row>
+    <row r="99" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
         <v>155</v>
       </c>
@@ -2831,8 +3750,12 @@
       <c r="F99" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="100" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G99">
+        <f>[1]Sheet1!B99</f>
+        <v>28048</v>
+      </c>
+    </row>
+    <row r="100" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
         <v>156</v>
       </c>
@@ -2851,8 +3774,12 @@
       <c r="F100" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="101" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G100">
+        <f>[1]Sheet1!B100</f>
+        <v>64336</v>
+      </c>
+    </row>
+    <row r="101" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
         <v>157</v>
       </c>

</xml_diff>